<commit_message>
add new map (subregions)
</commit_message>
<xml_diff>
--- a/data/maps_respin_wp1.xlsx
+++ b/data/maps_respin_wp1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" state="visible" r:id="rId4"/>
@@ -17,32 +17,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Country_name</t>
   </si>
   <si>
+    <t>IPBES_engagement</t>
+  </si>
+  <si>
+    <t>IPCC_engagement</t>
+  </si>
+  <si>
+    <t>Collaboration</t>
+  </si>
+  <si>
+    <t>IPCC_NFP_Org</t>
+  </si>
+  <si>
+    <t>IPBES_NFP_Org</t>
+  </si>
+  <si>
+    <t>IPBES_CB</t>
+  </si>
+  <si>
     <t>Category</t>
   </si>
   <si>
-    <t>IPBES_engagement</t>
-  </si>
-  <si>
-    <t>IPCC_engagement</t>
-  </si>
-  <si>
-    <t>Collaboration</t>
-  </si>
-  <si>
-    <t>IPCC_NFP_Org</t>
-  </si>
-  <si>
-    <t>IPBES_NFP_Org</t>
-  </si>
-  <si>
-    <t>IPBES_CB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Akrotiri and Dhekelia</t>
   </si>
   <si>
@@ -322,36 +322,36 @@
     <t xml:space="preserve">Same NFP</t>
   </si>
   <si>
+    <t xml:space="preserve">IPCC NFP's organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non applicable or unknown</t>
+  </si>
+  <si>
+    <t>#ffffb3</t>
+  </si>
+  <si>
+    <t>Ministery</t>
+  </si>
+  <si>
+    <t>#8dd3c7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Agency</t>
+  </si>
+  <si>
+    <t>#bebada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research agency and universities</t>
+  </si>
+  <si>
+    <t>#fb8072</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPBES NFP's organisation</t>
   </si>
   <si>
-    <t xml:space="preserve">Non applicable or unknown</t>
-  </si>
-  <si>
-    <t>#ffffb3</t>
-  </si>
-  <si>
-    <t>Ministery</t>
-  </si>
-  <si>
-    <t>#8dd3c7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Government Agency</t>
-  </si>
-  <si>
-    <t>#bebada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research agency and universities</t>
-  </si>
-  <si>
-    <t>#fb8072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPCC NFP's organisation</t>
-  </si>
-  <si>
     <t xml:space="preserve">IPBES Capacity building activities </t>
   </si>
   <si>
@@ -359,6 +359,18 @@
   </si>
   <si>
     <t xml:space="preserve">IPBES Capacity building activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World subregions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Asia</t>
   </si>
 </sst>
 </file>
@@ -997,19 +1009,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="I67" activeCellId="0" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="36.421875"/>
-    <col customWidth="1" min="2" max="2" style="1" width="8.90625"/>
-    <col customWidth="1" min="3" max="3" style="1" width="9.26953125"/>
-    <col customWidth="1" min="4" max="4" style="1" width="8.1796875"/>
-    <col customWidth="1" min="5" max="5" style="1" width="9.1796875"/>
-    <col min="6" max="6" style="1" width="10.90625"/>
-    <col customWidth="1" min="7" max="7" style="1" width="9.453125"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="17.51171875"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="16.6015625"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="12.82421875"/>
+    <col bestFit="1" min="5" max="5" style="1" width="13.40234375"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" style="1" width="14.3125"/>
+    <col bestFit="1" min="7" max="7" style="1" width="8.94140625"/>
     <col min="8" max="16384" style="1" width="10.90625"/>
   </cols>
   <sheetData>
@@ -1043,1720 +1055,1720 @@
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>3</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>2</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>3</v>
+      </c>
+      <c r="F13" s="4">
+        <v>3</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C13" s="4">
-        <v>3</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
-        <v>3</v>
-      </c>
-      <c r="G13" s="4">
-        <v>3</v>
-      </c>
-      <c r="H13" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>2</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="4">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C17" s="4">
-        <v>3</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4">
-        <v>2</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>2</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C20" s="1">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="1">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C21" s="1">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="1">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C23" s="1">
-        <v>3</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C24" s="1">
-        <v>3</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="1">
-        <v>2</v>
-      </c>
-      <c r="H24" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C25" s="1">
-        <v>3</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1">
-        <v>3</v>
-      </c>
-      <c r="G25" s="1">
-        <v>3</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C26" s="1">
-        <v>3</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1">
-        <v>2</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
-        <v>0</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C28" s="1">
-        <v>3</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1">
-        <v>1</v>
-      </c>
-      <c r="H28" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="1">
-        <v>2</v>
-      </c>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C30" s="1">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="1">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C31" s="1">
-        <v>3</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-      <c r="E31" s="1">
-        <v>1</v>
-      </c>
-      <c r="F31" s="1">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1">
-        <v>2</v>
-      </c>
-      <c r="H31" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="1">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C32" s="1">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-      <c r="G32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="1">
+        <v>3</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C33" s="1">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1">
-        <v>3</v>
-      </c>
-      <c r="G33" s="1">
-        <v>2</v>
-      </c>
-      <c r="H33" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="1">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C34" s="1">
-        <v>3</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1">
-        <v>2</v>
-      </c>
-      <c r="G34" s="1">
-        <v>2</v>
-      </c>
-      <c r="H34" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="1">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C35" s="1">
-        <v>2</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C37" s="1">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1</v>
-      </c>
-      <c r="E37" s="1">
-        <v>1</v>
-      </c>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
-      <c r="G37" s="1">
-        <v>0</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="1">
+        <v>3</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C38" s="1">
-        <v>3</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1</v>
-      </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1</v>
-      </c>
-      <c r="H38" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>2</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1">
-        <v>2</v>
-      </c>
-      <c r="G39" s="1">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="1">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C40" s="1">
-        <v>3</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1</v>
-      </c>
-      <c r="E40" s="1">
-        <v>2</v>
-      </c>
-      <c r="F40" s="1">
-        <v>1</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1</v>
-      </c>
-      <c r="H40" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="1">
+        <v>3</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C41" s="1">
-        <v>3</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1">
-        <v>2</v>
-      </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1">
-        <v>1</v>
-      </c>
-      <c r="H41" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-      <c r="F42" s="1">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="1">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C43" s="1">
-        <v>3</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1</v>
-      </c>
-      <c r="E43" s="1">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1">
-        <v>2</v>
-      </c>
-      <c r="H43" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="1">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C44" s="1">
-        <v>3</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1</v>
-      </c>
-      <c r="E44" s="1">
-        <v>2</v>
-      </c>
-      <c r="F44" s="1">
-        <v>1</v>
-      </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C45" s="1">
-        <v>2</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" s="1">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1">
-        <v>2</v>
-      </c>
-      <c r="G45" s="1">
-        <v>0</v>
-      </c>
-      <c r="H45" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C46" s="1">
-        <v>3</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
-      </c>
-      <c r="E46" s="1">
-        <v>1</v>
-      </c>
-      <c r="F46" s="1">
-        <v>1</v>
-      </c>
-      <c r="G46" s="1">
-        <v>1</v>
-      </c>
-      <c r="H46" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="1">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C47" s="1">
-        <v>3</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1">
-        <v>1</v>
-      </c>
-      <c r="F47" s="1">
-        <v>3</v>
-      </c>
-      <c r="G47" s="1">
-        <v>1</v>
-      </c>
-      <c r="H47" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
-      <c r="F48" s="1">
-        <v>1</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="1">
+        <v>3</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1">
+        <v>2</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C49" s="1">
-        <v>3</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" s="1">
-        <v>2</v>
-      </c>
-      <c r="F49" s="1">
-        <v>2</v>
-      </c>
-      <c r="G49" s="1">
-        <v>2</v>
-      </c>
-      <c r="H49" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="1">
+        <v>3</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50" s="1">
+        <v>3</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C50" s="1">
-        <v>3</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1">
-        <v>1</v>
-      </c>
-      <c r="F50" s="1">
-        <v>1</v>
-      </c>
-      <c r="G50" s="1">
-        <v>3</v>
-      </c>
-      <c r="H50" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="1">
+        <v>3</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C51" s="1">
-        <v>3</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
-      <c r="E51" s="1">
-        <v>1</v>
-      </c>
-      <c r="F51" s="1">
-        <v>2</v>
-      </c>
-      <c r="G51" s="1">
-        <v>3</v>
-      </c>
-      <c r="H51" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C52" s="1">
-        <v>3</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1</v>
-      </c>
-      <c r="E52" s="1">
-        <v>1</v>
-      </c>
-      <c r="F52" s="1">
-        <v>2</v>
-      </c>
-      <c r="G52" s="1">
-        <v>1</v>
-      </c>
-      <c r="H52" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="1">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1">
+        <v>3</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C53" s="1">
-        <v>3</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1">
-        <v>1</v>
-      </c>
-      <c r="F53" s="1">
-        <v>3</v>
-      </c>
-      <c r="G53" s="1">
-        <v>1</v>
-      </c>
-      <c r="H53" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1">
-        <v>1</v>
-      </c>
-      <c r="E54" s="1">
-        <v>1</v>
-      </c>
-      <c r="F54" s="1">
-        <v>3</v>
-      </c>
-      <c r="G54" s="1">
-        <v>0</v>
-      </c>
-      <c r="H54" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="1">
+        <v>3</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C55" s="1">
-        <v>3</v>
-      </c>
-      <c r="D55" s="1">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1">
-        <v>1</v>
-      </c>
-      <c r="F55" s="1">
-        <v>2</v>
-      </c>
-      <c r="G55" s="1">
-        <v>1</v>
-      </c>
-      <c r="H55" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="1">
+        <v>3</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C56" s="1">
-        <v>3</v>
-      </c>
-      <c r="D56" s="1">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1">
-        <v>2</v>
-      </c>
-      <c r="F56" s="1">
-        <v>1</v>
-      </c>
-      <c r="G56" s="1">
-        <v>1</v>
-      </c>
-      <c r="H56" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C57" s="1">
-        <v>1</v>
-      </c>
-      <c r="D57" s="1">
-        <v>1</v>
-      </c>
-      <c r="E57" s="1">
-        <v>2</v>
-      </c>
-      <c r="F57" s="1">
-        <v>1</v>
-      </c>
-      <c r="G57" s="1">
-        <v>1</v>
-      </c>
-      <c r="H57" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="1">
+        <v>3</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C58" s="1">
-        <v>3</v>
-      </c>
-      <c r="D58" s="1">
-        <v>1</v>
-      </c>
-      <c r="E58" s="1">
-        <v>2</v>
-      </c>
-      <c r="F58" s="1">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1">
-        <v>1</v>
-      </c>
-      <c r="H58" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="1">
+        <v>3</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2</v>
+      </c>
+      <c r="F59" s="1">
+        <v>2</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C59" s="1">
-        <v>3</v>
-      </c>
-      <c r="D59" s="1">
-        <v>1</v>
-      </c>
-      <c r="E59" s="1">
-        <v>2</v>
-      </c>
-      <c r="F59" s="1">
-        <v>2</v>
-      </c>
-      <c r="G59" s="1">
-        <v>2</v>
-      </c>
-      <c r="H59" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="1">
+        <v>3</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1">
+        <v>2</v>
+      </c>
+      <c r="F60" s="1">
+        <v>2</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C60" s="1">
-        <v>3</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" s="1">
-        <v>1</v>
-      </c>
-      <c r="F60" s="1">
-        <v>2</v>
-      </c>
-      <c r="G60" s="1">
-        <v>2</v>
-      </c>
-      <c r="H60" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="1">
+        <v>3</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C61" s="1">
-        <v>3</v>
-      </c>
-      <c r="D61" s="1">
-        <v>1</v>
-      </c>
-      <c r="E61" s="1">
-        <v>3</v>
-      </c>
-      <c r="F61" s="1">
-        <v>1</v>
-      </c>
-      <c r="G61" s="1">
-        <v>1</v>
-      </c>
-      <c r="H61" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="1">
+        <v>3</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2</v>
+      </c>
+      <c r="F62" s="1">
+        <v>2</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C62" s="1">
-        <v>3</v>
-      </c>
-      <c r="D62" s="1">
-        <v>1</v>
-      </c>
-      <c r="E62" s="1">
-        <v>1</v>
-      </c>
-      <c r="F62" s="1">
-        <v>2</v>
-      </c>
-      <c r="G62" s="1">
-        <v>2</v>
-      </c>
-      <c r="H62" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="1">
+        <v>3</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C63" s="1">
-        <v>3</v>
-      </c>
-      <c r="D63" s="1">
-        <v>1</v>
-      </c>
-      <c r="E63" s="1">
-        <v>1</v>
-      </c>
-      <c r="F63" s="1">
-        <v>1</v>
-      </c>
-      <c r="G63" s="1">
-        <v>1</v>
-      </c>
-      <c r="H63" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
-      <c r="D64" s="1">
-        <v>1</v>
-      </c>
-      <c r="E64" s="1">
-        <v>1</v>
-      </c>
-      <c r="F64" s="1">
-        <v>1</v>
-      </c>
-      <c r="G64" s="1">
-        <v>0</v>
-      </c>
-      <c r="H64" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1">
+        <v>1</v>
+      </c>
+      <c r="E65" s="1">
+        <v>2</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1">
-        <v>1</v>
-      </c>
-      <c r="E65" s="1">
-        <v>1</v>
-      </c>
-      <c r="F65" s="1">
-        <v>2</v>
-      </c>
-      <c r="G65" s="1">
-        <v>0</v>
-      </c>
-      <c r="H65" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="1">
+        <v>3</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1">
+        <v>1</v>
+      </c>
+      <c r="E66" s="1">
+        <v>2</v>
+      </c>
+      <c r="F66" s="1">
+        <v>2</v>
+      </c>
+      <c r="G66" s="1">
+        <v>1</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C66" s="1">
-        <v>3</v>
-      </c>
-      <c r="D66" s="1">
-        <v>1</v>
-      </c>
-      <c r="E66" s="1">
-        <v>1</v>
-      </c>
-      <c r="F66" s="1">
-        <v>2</v>
-      </c>
-      <c r="G66" s="1">
-        <v>2</v>
-      </c>
-      <c r="H66" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="1">
+        <v>3</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1">
+        <v>1</v>
+      </c>
+      <c r="E67" s="1">
+        <v>2</v>
+      </c>
+      <c r="F67" s="1">
+        <v>2</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C67" s="1">
-        <v>3</v>
-      </c>
-      <c r="D67" s="1">
-        <v>1</v>
-      </c>
-      <c r="E67" s="1">
-        <v>1</v>
-      </c>
-      <c r="F67" s="1">
-        <v>2</v>
-      </c>
-      <c r="G67" s="1">
-        <v>2</v>
-      </c>
-      <c r="H67" s="1">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G68">
+  <sortState ref="A2:F68">
     <sortCondition ref="A7"/>
   </sortState>
   <printOptions headings="0" gridLines="0"/>
@@ -3153,23 +3165,56 @@
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="6">
+        <v>7</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
+      <c r="A23" s="6">
+        <v>7</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="6">
+        <v>7</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="6"/>

</xml_diff>